<commit_message>
Uploading updated test cases.
</commit_message>
<xml_diff>
--- a/GameTestCases.xlsx
+++ b/GameTestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.bowen\source\repos\Kanrail\5153-Ethics_Game\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.bowen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62AFB8F0-7FD2-4290-AB5A-665D1B3C1C7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E36CF82-D5C8-4EE3-9016-0CE40FE37F70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="166">
   <si>
     <t>Feature</t>
   </si>
@@ -112,19 +112,436 @@
   </si>
   <si>
     <t>Hard Button Press</t>
+  </si>
+  <si>
+    <t>Snake MG</t>
+  </si>
+  <si>
+    <t>Displays correctly after game loss</t>
+  </si>
+  <si>
+    <t>Game Over Screen</t>
+  </si>
+  <si>
+    <t>GO Restart Button Hover</t>
+  </si>
+  <si>
+    <t>GO Restart Button Press</t>
+  </si>
+  <si>
+    <t>GO Main Menu Button Hover</t>
+  </si>
+  <si>
+    <t>GO Main Menu Button Press</t>
+  </si>
+  <si>
+    <t>Darkens to a slight grey on mouse hover</t>
+  </si>
+  <si>
+    <t>Darkens to almost black and then Redirects player to main menu</t>
+  </si>
+  <si>
+    <t>Darkens to almost black and then restarts the snake game from beginning</t>
+  </si>
+  <si>
+    <t>Game correctly ends and proceeds to next scene upon reaching 0 pellets</t>
+  </si>
+  <si>
+    <t>ball starts moving</t>
+  </si>
+  <si>
+    <t>right bar moves up</t>
+  </si>
+  <si>
+    <t>right bar moves down</t>
+  </si>
+  <si>
+    <t>left bar moves up</t>
+  </si>
+  <si>
+    <t>left bar moves down</t>
+  </si>
+  <si>
+    <t>Pong Game</t>
+  </si>
+  <si>
+    <t>Scene Start: Pellet Spawn</t>
+  </si>
+  <si>
+    <t>Scene Start: Snake Starts Moving</t>
+  </si>
+  <si>
+    <t>Single pellet starts on screen and food pellets start randomly appearing within the white boundaries</t>
+  </si>
+  <si>
+    <t>Snake starts moving to right</t>
+  </si>
+  <si>
+    <t>Snake Collision: Food Pellet</t>
+  </si>
+  <si>
+    <t>Snake Collision: Top Border</t>
+  </si>
+  <si>
+    <t>Snake Collision: Bottom Border</t>
+  </si>
+  <si>
+    <t>Snake Collision: Left Border</t>
+  </si>
+  <si>
+    <t>Snake Collision: Right Border</t>
+  </si>
+  <si>
+    <t>Game shifts to game over screen</t>
+  </si>
+  <si>
+    <t>Snake Collision: Tail</t>
+  </si>
+  <si>
+    <t>Food pellet disappears, snake grows by one tail piece, score counter decreased by 1</t>
+  </si>
+  <si>
+    <t>Snake Movement: Up key pressed</t>
+  </si>
+  <si>
+    <t>Snake Movement: Down key pressed</t>
+  </si>
+  <si>
+    <t>Snake Movement: Left key pressed</t>
+  </si>
+  <si>
+    <t>Snake Movement: Right key pressed</t>
+  </si>
+  <si>
+    <t>Snake starts moving down, tail follows at pivot point</t>
+  </si>
+  <si>
+    <t>Snake starts moving right, tail follows at pivot point</t>
+  </si>
+  <si>
+    <t>Snake starts moving left, tail follows at pivot point</t>
+  </si>
+  <si>
+    <t>Snake starts moving up, tail follows at pivot point</t>
+  </si>
+  <si>
+    <t>Score counter initializes to 10 (default for now)</t>
+  </si>
+  <si>
+    <t>Scene Start: Score Counter Initializes</t>
+  </si>
+  <si>
+    <t>Score Counter Updated</t>
+  </si>
+  <si>
+    <t>Accurately displays remaining pellets needed</t>
+  </si>
+  <si>
+    <t>Score counter reaches 0</t>
+  </si>
+  <si>
+    <t>Start game button hover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End game button hover </t>
+  </si>
+  <si>
+    <t>Start game button press</t>
+  </si>
+  <si>
+    <t>switch to pong game scene</t>
+  </si>
+  <si>
+    <t>End game button press</t>
+  </si>
+  <si>
+    <t>switch to main menu</t>
+  </si>
+  <si>
+    <t>Scene starts player waits 2.5 seconds</t>
+  </si>
+  <si>
+    <t>Press up arrow key</t>
+  </si>
+  <si>
+    <t>Press down arrow key</t>
+  </si>
+  <si>
+    <t>Press w key</t>
+  </si>
+  <si>
+    <t>Press s key</t>
+  </si>
+  <si>
+    <t>Ball hits on top border</t>
+  </si>
+  <si>
+    <t>ball bounces down at an angle same direction in which it hit</t>
+  </si>
+  <si>
+    <t>Ball hits on bottom border</t>
+  </si>
+  <si>
+    <t>ball bounces up at an angle same direction in which it hit</t>
+  </si>
+  <si>
+    <t>Ball hits on left bar</t>
+  </si>
+  <si>
+    <t>ball moves in opposite direction randomly</t>
+  </si>
+  <si>
+    <t>Ball hits on right bar</t>
+  </si>
+  <si>
+    <t>Ball miss to hit on right bar</t>
+  </si>
+  <si>
+    <t>displays game over with which player wins</t>
+  </si>
+  <si>
+    <t>Ball miss to hit on left bar</t>
+  </si>
+  <si>
+    <t>Player 1 win screen</t>
+  </si>
+  <si>
+    <t>screen displays if player1 wins</t>
+  </si>
+  <si>
+    <t>Player 2 win screen</t>
+  </si>
+  <si>
+    <t>screen displays if player2 wins</t>
+  </si>
+  <si>
+    <t>Player 1 screen rematch button hover</t>
+  </si>
+  <si>
+    <t>Player 2 screen rematch button hover</t>
+  </si>
+  <si>
+    <t>Player 1 screen rematch button press</t>
+  </si>
+  <si>
+    <t>Player 2 screen rematch button press</t>
+  </si>
+  <si>
+    <t>Bird Game</t>
+  </si>
+  <si>
+    <t>Game starts when user clicks spacebar</t>
+  </si>
+  <si>
+    <t>Game Start</t>
+  </si>
+  <si>
+    <t>Bird by default falls down</t>
+  </si>
+  <si>
+    <t>If nothing is input by the user, the bird natrually falls</t>
+  </si>
+  <si>
+    <t>Game Over by Ground Collision</t>
+  </si>
+  <si>
+    <t>Game restarts if bird collides with ground</t>
+  </si>
+  <si>
+    <t>Game Over by Log Collision</t>
+  </si>
+  <si>
+    <t>Game restarts if bird collides with a log</t>
+  </si>
+  <si>
+    <t>Logs move up and down</t>
+  </si>
+  <si>
+    <t>When the user presses the spacebar, the bird flies up a short distance</t>
+  </si>
+  <si>
+    <t>Game win</t>
+  </si>
+  <si>
+    <t>Game recognizes when bird touches/passes green line (the goal)</t>
+  </si>
+  <si>
+    <t>Press Spacebar</t>
+  </si>
+  <si>
+    <t>Bird Sprite Animation</t>
+  </si>
+  <si>
+    <t>Animation of bird flapping starts at scene start</t>
+  </si>
+  <si>
+    <t>Goal line Collision</t>
+  </si>
+  <si>
+    <t>Proceeds to next scene</t>
+  </si>
+  <si>
+    <t>Logs move up and down at scene start</t>
+  </si>
+  <si>
+    <t>Player 1 screen EndGame button press</t>
+  </si>
+  <si>
+    <t>Player 2 screen EndGame button hover</t>
+  </si>
+  <si>
+    <t>Player 1 screen EndGame button hover</t>
+  </si>
+  <si>
+    <t>Player 2 screen EndGame button press</t>
+  </si>
+  <si>
+    <t>Restarts the pong game scene</t>
+  </si>
+  <si>
+    <t>Wireframing</t>
+  </si>
+  <si>
+    <t>Level Select Easy Button Press</t>
+  </si>
+  <si>
+    <t>Level Select Medium Button Press</t>
+  </si>
+  <si>
+    <t>Level Select Hard Button Press</t>
+  </si>
+  <si>
+    <t>Proceeds to Snake minigame scene</t>
+  </si>
+  <si>
+    <t>Proceeds to Pong minigame scene</t>
+  </si>
+  <si>
+    <t>Proceeds to Flappybird minigame scene</t>
+  </si>
+  <si>
+    <t>Start Screen Help Button Press</t>
+  </si>
+  <si>
+    <t>Start Screen Credits Button Press</t>
+  </si>
+  <si>
+    <t>Proceeds to Help scene</t>
+  </si>
+  <si>
+    <t>Proceeds to Credits scene</t>
+  </si>
+  <si>
+    <t>Pong P1 Win End Game Button Press</t>
+  </si>
+  <si>
+    <t>Pong P2 Win End Game Button Press</t>
+  </si>
+  <si>
+    <t>Proceeds to Ethics Question scene</t>
+  </si>
+  <si>
+    <t>Snake Game Win</t>
+  </si>
+  <si>
+    <t>Help Screen Back Button Press</t>
+  </si>
+  <si>
+    <t>Credits Screen Back Button Press</t>
+  </si>
+  <si>
+    <t>Proceeds to Main Menu scene</t>
+  </si>
+  <si>
+    <t>Ethics Question</t>
+  </si>
+  <si>
+    <t>Question Populates</t>
+  </si>
+  <si>
+    <t>Answer Labels Populate</t>
+  </si>
+  <si>
+    <t>Incorrect Answer Button Press</t>
+  </si>
+  <si>
+    <t>Correct Answer Button Press</t>
+  </si>
+  <si>
+    <t>Win Screen Next Button Press</t>
+  </si>
+  <si>
+    <t>Lose Screen Next Button Press</t>
+  </si>
+  <si>
+    <t>Question populates with randomly chosen question from file</t>
+  </si>
+  <si>
+    <t>Answers populate that associate to chosen question from file</t>
+  </si>
+  <si>
+    <t>Incorrect answer clicked takes you to the Lose scene</t>
+  </si>
+  <si>
+    <t>Correct answer clicked takes you to the Win scene</t>
+  </si>
+  <si>
+    <t>Next takes you back to the main menu</t>
+  </si>
+  <si>
+    <t>Question Dictionary Populates</t>
+  </si>
+  <si>
+    <t>Behind scenes, question dictionary populates with question and answers</t>
+  </si>
+  <si>
+    <t>Top-left button hover</t>
+  </si>
+  <si>
+    <t>Top-left button press</t>
+  </si>
+  <si>
+    <t>Top-right button hover</t>
+  </si>
+  <si>
+    <t>Top-right button press</t>
+  </si>
+  <si>
+    <t>Bottom-left button hover</t>
+  </si>
+  <si>
+    <t>Bottom-left button press</t>
+  </si>
+  <si>
+    <t>Bottom right button hover</t>
+  </si>
+  <si>
+    <t>Bottem right button press</t>
+  </si>
+  <si>
+    <t>Button highlights with light shade</t>
+  </si>
+  <si>
+    <t>Button highlights with a darker shade until release</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,8 +564,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -209,7 +630,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -261,7 +682,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -463,17 +884,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -663,7 +1087,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>15</v>
       </c>
@@ -674,7 +1098,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>16</v>
       </c>
@@ -685,12 +1109,923 @@
         <v>10</v>
       </c>
     </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
+      <c r="C45" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>88</v>
+      </c>
+      <c r="D53" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D54" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>91</v>
+      </c>
+      <c r="D55" t="s">
+        <v>90</v>
+      </c>
+      <c r="E55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" t="s">
+        <v>93</v>
+      </c>
+      <c r="E56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>94</v>
+      </c>
+      <c r="D57" t="s">
+        <v>95</v>
+      </c>
+      <c r="E57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" t="s">
+        <v>36</v>
+      </c>
+      <c r="E58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>121</v>
+      </c>
+      <c r="D59" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>97</v>
+      </c>
+      <c r="D60" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>98</v>
+      </c>
+      <c r="D62" t="s">
+        <v>123</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>119</v>
+      </c>
+      <c r="D63" t="s">
+        <v>117</v>
+      </c>
+      <c r="E63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>99</v>
+      </c>
+      <c r="D64" t="s">
+        <v>123</v>
+      </c>
+      <c r="E64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>122</v>
+      </c>
+      <c r="D65" t="s">
+        <v>117</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>3</v>
+      </c>
+      <c r="B67" t="s">
+        <v>100</v>
+      </c>
+      <c r="C67" t="s">
+        <v>102</v>
+      </c>
+      <c r="D67" t="s">
+        <v>101</v>
+      </c>
+      <c r="E67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>103</v>
+      </c>
+      <c r="D68" t="s">
+        <v>104</v>
+      </c>
+      <c r="E68" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>105</v>
+      </c>
+      <c r="D69" t="s">
+        <v>106</v>
+      </c>
+      <c r="E69" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>107</v>
+      </c>
+      <c r="D70" t="s">
+        <v>108</v>
+      </c>
+      <c r="E70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>114</v>
+      </c>
+      <c r="D71" t="s">
+        <v>115</v>
+      </c>
+      <c r="E71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>109</v>
+      </c>
+      <c r="D72" t="s">
+        <v>118</v>
+      </c>
+      <c r="E72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>113</v>
+      </c>
+      <c r="D73" t="s">
+        <v>110</v>
+      </c>
+      <c r="E73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D74" t="s">
+        <v>112</v>
+      </c>
+      <c r="E74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>116</v>
+      </c>
+      <c r="D75" t="s">
+        <v>137</v>
+      </c>
+      <c r="E75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>3</v>
+      </c>
+      <c r="B77" t="s">
+        <v>124</v>
+      </c>
+      <c r="C77" t="s">
+        <v>125</v>
+      </c>
+      <c r="D77" t="s">
+        <v>128</v>
+      </c>
+      <c r="E77" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>126</v>
+      </c>
+      <c r="D78" t="s">
+        <v>129</v>
+      </c>
+      <c r="E78" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>127</v>
+      </c>
+      <c r="D79" t="s">
+        <v>130</v>
+      </c>
+      <c r="E79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>131</v>
+      </c>
+      <c r="D80" t="s">
+        <v>133</v>
+      </c>
+      <c r="E80" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>132</v>
+      </c>
+      <c r="D81" t="s">
+        <v>134</v>
+      </c>
+      <c r="E81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>135</v>
+      </c>
+      <c r="D82" t="s">
+        <v>137</v>
+      </c>
+      <c r="E82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>136</v>
+      </c>
+      <c r="D83" t="s">
+        <v>137</v>
+      </c>
+      <c r="E83" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>138</v>
+      </c>
+      <c r="D84" t="s">
+        <v>137</v>
+      </c>
+      <c r="E84" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>139</v>
+      </c>
+      <c r="D85" t="s">
+        <v>141</v>
+      </c>
+      <c r="E85" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>140</v>
+      </c>
+      <c r="D86" t="s">
+        <v>141</v>
+      </c>
+      <c r="E86" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>3</v>
+      </c>
+      <c r="B88" t="s">
+        <v>142</v>
+      </c>
+      <c r="C88" t="s">
+        <v>143</v>
+      </c>
+      <c r="D88" t="s">
+        <v>149</v>
+      </c>
+      <c r="E88" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>144</v>
+      </c>
+      <c r="D89" t="s">
+        <v>150</v>
+      </c>
+      <c r="E89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>145</v>
+      </c>
+      <c r="D90" t="s">
+        <v>151</v>
+      </c>
+      <c r="E90" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>146</v>
+      </c>
+      <c r="D91" t="s">
+        <v>152</v>
+      </c>
+      <c r="E91" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>147</v>
+      </c>
+      <c r="D92" t="s">
+        <v>153</v>
+      </c>
+      <c r="E92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>148</v>
+      </c>
+      <c r="D93" t="s">
+        <v>153</v>
+      </c>
+      <c r="E93" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>154</v>
+      </c>
+      <c r="D94" t="s">
+        <v>155</v>
+      </c>
+      <c r="E94" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>156</v>
+      </c>
+      <c r="D95" t="s">
+        <v>164</v>
+      </c>
+      <c r="E95" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>157</v>
+      </c>
+      <c r="D96" t="s">
+        <v>165</v>
+      </c>
+      <c r="E96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>158</v>
+      </c>
+      <c r="D97" t="s">
+        <v>164</v>
+      </c>
+      <c r="E97" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>159</v>
+      </c>
+      <c r="D98" t="s">
+        <v>165</v>
+      </c>
+      <c r="E98" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>160</v>
+      </c>
+      <c r="D99" t="s">
+        <v>164</v>
+      </c>
+      <c r="E99" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>161</v>
+      </c>
+      <c r="D100" t="s">
+        <v>165</v>
+      </c>
+      <c r="E100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>162</v>
+      </c>
+      <c r="D101" t="s">
+        <v>164</v>
+      </c>
+      <c r="E101" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>163</v>
+      </c>
+      <c r="D102" t="s">
+        <v>165</v>
+      </c>
+      <c r="E102" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002F3B64CF3F87534C89394D192F37FE03" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bc92f62612f157ce92826da6fac2f568">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1a853a03-70b7-4e88-b9d6-862a6d0d513b" xmlns:ns4="006257e6-8004-434d-9d5c-8648ed86a46d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53f9340ff9bd35e08117073a0c9a3ff6" ns3:_="" ns4:_="">
     <xsd:import namespace="1a853a03-70b7-4e88-b9d6-862a6d0d513b"/>
@@ -913,15 +2248,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -929,6 +2255,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB8A67A2-5DDB-4C40-88B1-8FE14C708844}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E9AF1B-1443-4248-BC04-1FB939548151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -947,19 +2281,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB8A67A2-5DDB-4C40-88B1-8FE14C708844}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A76F575D-EE7F-4E8F-A345-86B9CCF1C624}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="006257e6-8004-434d-9d5c-8648ed86a46d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a853a03-70b7-4e88-b9d6-862a6d0d513b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>